<commit_message>
update files to console
</commit_message>
<xml_diff>
--- a/console/Networking/iaas-network/aclMixinsXlsx/acl_list.xlsx
+++ b/console/Networking/iaas-network/aclMixinsXlsx/acl_list.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\han\Desktop\京东云-返工\18. ACL国际化内容翻译确认\4. 确认后-柴玉梅\2. 客户确认后-上传Github版\ACL国际化内容翻译确认-CT-C-GTCOM Comment1106-R\aclMixinsXlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="20730" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="ch" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -636,18 +641,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>确认删除网络ACL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>acl_list_i18nKey_27</t>
     </r>
   </si>
@@ -684,30 +677,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>'删除公网IP成功</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Network ACL Help Documentation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Create</t>
     </r>
   </si>
@@ -732,30 +701,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Hosting VPC</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Associate Subnet</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Creation Time</t>
     </r>
   </si>
@@ -816,18 +761,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>No Network ACL Data</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>‘Clone ACL’</t>
     </r>
   </si>
@@ -876,66 +809,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>‘Begin to Get ACL list’</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>‘ACL list data are</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>‘Begin to Get VPC Drop-down List’</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>‘VPC Drop-down List Data are</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>‘After creating network ACL, you need to set inbound and outbound rules and associate them to the subnet for coming into effect’</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>'Notification'</t>
     </r>
   </si>
@@ -973,18 +846,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>‘ACL is associated with the subnet successfully’</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Confirm to Delete Network ACL</t>
     </r>
   </si>
   <si>
@@ -1004,15 +865,273 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>‘Deleted Public IP</t>
+    <t>Associate Subnet</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Network ACL Help Documentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>No Network ACL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> data</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACL lists are</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VPC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">‘Begin to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> VPC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> drop-down lists</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>’</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Begin to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">get </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ACL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lists</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>‘VPC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> drop-down</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">lists  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>are</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">‘After creating </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Network</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ACL, you need to set inbound and outbound rules and associate the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ACL with a subnet so that the Network ACL can take effect to protect the security of the subnet'</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>确认删除网络</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ACL</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>删除公网</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Public IP deleted </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Confirm to delete Network ACL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1022,6 +1141,29 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1048,9 +1190,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1394,18 +1548,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.21875" customWidth="1"/>
-    <col min="2" max="2" width="42.33203125" customWidth="1"/>
-    <col min="3" max="3" width="54.77734375" customWidth="1"/>
+    <col min="2" max="2" width="29.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1413,7 +1567,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1424,7 +1578,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1435,7 +1589,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1446,7 +1600,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1456,8 +1610,8 @@
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>59</v>
+      <c r="C5" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1468,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1479,7 +1633,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1490,7 +1644,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1501,10 +1655,10 @@
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1512,7 +1666,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1523,7 +1677,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1534,7 +1688,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1545,7 +1699,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1556,7 +1710,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1567,7 +1721,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1578,7 +1732,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1589,7 +1743,7 @@
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1599,8 +1753,8 @@
       <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>72</v>
+      <c r="C18" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1611,7 +1765,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1622,10 +1776,10 @@
         <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1633,7 +1787,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1644,7 +1798,7 @@
         <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1655,7 +1809,7 @@
         <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1666,10 +1820,10 @@
         <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1677,40 +1831,40 @@
         <v>49</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="5" t="s">
         <v>80</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>83</v>
+        <v>53</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1718,7 +1872,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B28" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B25 A28 A27:B27 A26" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>